<commit_message>
Modify zip password or windows. CHECK LINUX.
</commit_message>
<xml_diff>
--- a/system_template/data/en/mail_template.xlsx
+++ b/system_template/data/en/mail_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Dropbox\3_Develop\TFS_Exc\ExmentProject\vendor\exceedone\exment\system_template\data\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A030635-F093-4D96-BC80-C985946F9C70}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC08195-87E8-4106-AAF7-C2AF18937949}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25335" yWindow="180" windowWidth="25470" windowHeight="15420" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
   </bookViews>
   <sheets>
     <sheet name="mail_template" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -202,6 +202,17 @@
   </si>
   <si>
     <t>Sent to the person who logged in with ID/password.\nRegister Google 2-step verification.\n\n[Registration URL]\n${2factor_google_register_url}\n[expiration date]\n${valid_period_datetime}\n\n* If you do not remember logging in but received this email, your account may have been used illegally. We recommend that you change your password.\n* If the expiration date has expired, please enter your ID/password again to log in.</t>
+  </si>
+  <si>
+    <t>password_notify_header</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[${system:site_name}]Password notification header</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>***************************************************************************\nThis email is automatically encrypted as an attachment.\nYou will receive a password from the sender later.\n***************************************************************************\n\n</t>
   </si>
 </sst>
 </file>
@@ -568,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C02B19E-36B6-49DD-989B-C96CC8D7F9C4}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -804,6 +815,23 @@
         <v>50</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug fix mail templdate attachment and comment wrong target
</commit_message>
<xml_diff>
--- a/system_template/data/en/mail_template.xlsx
+++ b/system_template/data/en/mail_template.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Dropbox\3_Develop\TFS_Exc\ExmentProject2\vendor\exceedone\exment\system_template\data\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h-sat\Dropbox\3_Develop\TFS_Exc\ExmentProject2\vendor\exceedone\exment\system_template\data\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818AFB11-BB6B-4E66-BEF6-AEE42D0E1679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF44B9DE-0E03-480C-8AE3-BE069FF375EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
   </bookViews>
   <sheets>
     <sheet name="mail_template" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -189,10 +198,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Data for ${target_table} has been ${create_or_update} by user ${updated_user}.\nPlease check the following.\n\n${create_or_update} User: ${target_user}\n${create_or_update} Date: ${target_datetime}\n${create_or_update} Data: ${value_url/link=true}\n${free_space}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Sent to the person who logged in with ID/password.\n\n[authentication code]\n${verify_code}\n[expiration date]\n${valid_period_datetime}\n\n*If you do not remember logging in but received this email, your account may have been used illegally. We recommend that you change your password.\n*If the expiration date has expired, please enter your ID/password again to log in.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -212,6 +217,10 @@
   </si>
   <si>
     <t>The notification date set by the system for the data registered in ${system:site_name} has been reached. Please check the contents after login.\n\n[registered content]\n-Notification name:${notify:notify_view_name}\n-Target table:${target_table}\n-Target data:${value_url/link=true}\n・ ${Notify_target_column_key}:${notify_target_column_value}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data for ${target_table} has been ${create_or_update} by user ${target_user}.\nPlease check the following.\n\n${create_or_update} User: ${target_user}\n${create_or_update} Date: ${target_datetime}\n${create_or_update} Data: ${value_url/link=true}\n${free_space}</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -582,12 +591,12 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -627,7 +636,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -647,7 +656,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -667,7 +676,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>3</v>
       </c>
@@ -687,7 +696,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>4</v>
       </c>
@@ -707,7 +716,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>5</v>
       </c>
@@ -724,10 +733,10 @@
         <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>6</v>
       </c>
@@ -744,10 +753,10 @@
         <v>39</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -761,10 +770,10 @@
         <v>40</v>
       </c>
       <c r="F9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -778,10 +787,10 @@
         <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -798,7 +807,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>24</v>
       </c>
@@ -815,9 +824,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
@@ -826,10 +835,10 @@
         <v>23</v>
       </c>
       <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" t="s">
         <v>54</v>
-      </c>
-      <c r="F13" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add initial data to infomation,mail template
</commit_message>
<xml_diff>
--- a/system_template/data/en/mail_template.xlsx
+++ b/system_template/data/en/mail_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\h-sat\Dropbox\3_Develop\TFS_Exc\ExmentProject2\vendor\exceedone\exment\system_template\data\en\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\exment_eng\vendor\exceedone\exment\system_template\data\en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF44B9DE-0E03-480C-8AE3-BE069FF375EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126CFBE9-EE4D-4748-A2B0-FE765D6975A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
+    <workbookView xWindow="5400" yWindow="2955" windowWidth="21120" windowHeight="11865" xr2:uid="{D6B672C1-A825-47CF-A377-E0B53872B948}"/>
   </bookViews>
   <sheets>
     <sheet name="mail_template" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -221,6 +221,70 @@
   </si>
   <si>
     <t>Data for ${target_table} has been ${create_or_update} by user ${target_user}.\nPlease check the following.\n\n${create_or_update} User: ${target_user}\n${create_or_update} Date: ${target_datetime}\n${create_or_update} Data: ${value_url/link=true}\n${free_space}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>workflow_notify</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>publicform_complete_user</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>publicform_complete_admin</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>publicform_error</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Workflow execution</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Public form completion notification (general user)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Public form completion notification (administrator)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Public form error notification (administrator)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[${system:site_name}]Input is complete</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[${system:site_name}]Workflow ${workflow_action} has been executed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[${system:site_name}]Input was made on public form ${publicform:public_form_view_name}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[${system:site_name}]Some errors occurred on public form ${publicform:public_form_view_name}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To ${user:user_name}\n\n${workflow:action_name} has been executed by ${workflow:action_user}.\nCheck the data and what was done, and then take the following actions.\n\nTarget data : ${value_url/link=true}\nData creation user : ${created_user}\nExecuted action : ${workflow:action_name}\nAction execution user : ${workflow:action_user}\nCurrent Status : ${workflow:status_name}\n\nComment : \n${workflow:comment}\n\n</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Thank you for your input. \nInput is complete. Please check your input.\n\n*Input data\n${publicform:inputs}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To ${user:user_name}\n\nYou have entered the data for the public form ${publicform:public_form_view_name}.\nPlease check the entered data.\n\n*Input data\n${publicform:inputs}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To ${user:user_name}\n\nSome errors occurred while filling out the public form ${publicform:public_form_view_name}.\nPlease check the entered contents and the error contents.\n\n*Input data\n${publicform:inputs}\n\n*Error summary\n${error:message}\n\n*Error detail\n${error:stacktrace}\n\n</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -588,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C02B19E-36B6-49DD-989B-C96CC8D7F9C4}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -841,6 +905,74 @@
         <v>54</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" t="s">
+        <v>23</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>